<commit_message>
test of cmu and union square
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,49 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7234A59-8BBD-9447-8091-6890CBA96203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21820CF2-7331-A847-A774-3539B82A3043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="540" windowWidth="25440" windowHeight="14400" xr2:uid="{B61788FE-B626-4F4E-8DEB-0C7704611D16}"/>
+    <workbookView xWindow="3300" yWindow="460" windowWidth="25440" windowHeight="14400" xr2:uid="{B61788FE-B626-4F4E-8DEB-0C7704611D16}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BSD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$4:$I$4</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$5:$I$5</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$6:$I$6</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$7:$I$7</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$B$8:$I$8</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$9:$I$9</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$2</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$3:$A$9</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$3:$B$9</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$C$2</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$3:$C$9</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$D$2</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$3:$D$9</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$E$3:$E$9</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$F$2</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$F$3:$F$9</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$G$2</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$G$3:$G$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$H$2</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$H$3:$H$9</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$I$2</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$I$3:$I$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$7</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$8</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$9</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$2:$I$2</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$3:$I$3</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,9 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>wall street</t>
+    <t>wall street with turns</t>
+  </si>
+  <si>
+    <t>union square with turns</t>
+  </si>
+  <si>
+    <t>cmu with turns</t>
   </si>
 </sst>
 </file>
@@ -128,7 +98,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,7 +203,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>BSD!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -254,7 +226,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:f>BSD!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -287,7 +259,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$I$3</c:f>
+              <c:f>BSD!$B$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -330,7 +302,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>BSD!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -353,7 +325,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:f>BSD!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -386,7 +358,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$I$4</c:f>
+              <c:f>BSD!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -429,7 +401,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>BSD!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -452,7 +424,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:f>BSD!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -485,7 +457,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$I$5</c:f>
+              <c:f>BSD!$B$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -528,7 +500,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>BSD!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -551,7 +523,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:f>BSD!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -584,7 +556,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$I$6</c:f>
+              <c:f>BSD!$B$6:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -627,7 +599,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>BSD!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -650,7 +622,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:f>BSD!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -683,7 +655,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$I$7</c:f>
+              <c:f>BSD!$B$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -726,7 +698,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>BSD!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -749,7 +721,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:f>BSD!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -782,7 +754,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$I$8</c:f>
+              <c:f>BSD!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -825,7 +797,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>BSD!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -850,7 +822,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:f>BSD!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -883,7 +855,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$I$9</c:f>
+              <c:f>BSD!$B$9:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1117,7 +1089,2037 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>union</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> square</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$19:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23599999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FA2B-604F-93B2-68C38EA564CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$20:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64800000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FA2B-604F-93B2-68C38EA564CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88800000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FA2B-604F-93B2-68C38EA564CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$22:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96399999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FA2B-604F-93B2-68C38EA564CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$23:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80200000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FA2B-604F-93B2-68C38EA564CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$24:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92200000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-FA2B-604F-93B2-68C38EA564CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$25:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.378</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83399999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99199999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-FA2B-604F-93B2-68C38EA564CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="442669936"/>
+        <c:axId val="441360000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="442669936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441360000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="441360000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="442669936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>cmu</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$35:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.218</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6138-4F41-8D36-9D33E3F8808E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$36:$I$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41799999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6138-4F41-8D36-9D33E3F8808E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$37:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74199999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6138-4F41-8D36-9D33E3F8808E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$38:$I$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6138-4F41-8D36-9D33E3F8808E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$39:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6138-4F41-8D36-9D33E3F8808E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$40:$I$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92600000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6138-4F41-8D36-9D33E3F8808E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD!$B$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.25600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.874</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94199999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-6138-4F41-8D36-9D33E3F8808E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="414937120"/>
+        <c:axId val="415217552"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="414937120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="415217552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="415217552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414937120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1673,6 +3675,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1706,6 +4740,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCC54C9C-EE58-2543-A6EE-DAC875E855B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00E87ADF-893D-D947-93D8-D4F176546198}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2011,22 +5117,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0696D5-A371-9F4F-BB99-FEDCE10E8E3F}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -2261,7 +5367,506 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2">
+        <v>20</v>
+      </c>
+      <c r="F18" s="2">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2">
+        <v>30</v>
+      </c>
+      <c r="H18" s="2">
+        <v>35</v>
+      </c>
+      <c r="I18" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.23599999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.112</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.316</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.64800000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>70</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>75</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.96399999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>80</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>90</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.378</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.998</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.998</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.996</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="2">
+        <v>5</v>
+      </c>
+      <c r="C34" s="2">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2">
+        <v>15</v>
+      </c>
+      <c r="E34" s="2">
+        <v>20</v>
+      </c>
+      <c r="F34" s="2">
+        <v>25</v>
+      </c>
+      <c r="G34" s="2">
+        <v>30</v>
+      </c>
+      <c r="H34" s="2">
+        <v>35</v>
+      </c>
+      <c r="I34" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>50</v>
+      </c>
+      <c r="B35" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>60</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>70</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>75</v>
+      </c>
+      <c r="B38" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.746</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>80</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.224</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.628</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>90</v>
+      </c>
+      <c r="B40" s="1">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.92600000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>100</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.874</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.94199999999999995</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A33:I33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
find out the difference between real and simulated
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9985572-CAB4-A74F-93AD-9E9FD939B0A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0CBB1A-1FA0-C949-A0C2-08CB40CD6099}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="460" windowWidth="24700" windowHeight="14220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="24700" windowHeight="14220" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSD_T_length " sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>wall street with turns (new test routes)</t>
   </si>
@@ -1216,28 +1216,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.2000000000000003E-2</c:v>
+                  <c:v>3.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31</c:v>
+                  <c:v>0.35199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.66200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77800000000000002</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86399999999999999</c:v>
+                  <c:v>0.89800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.93200000000000005</c:v>
+                  <c:v>0.94199999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.95799999999999996</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96</c:v>
+                  <c:v>0.95199999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1752,6 +1752,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.216</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.434</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92600000000000005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1827,6 +1851,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95399999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1902,6 +1950,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.14399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97799999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1977,6 +2049,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.35799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2054,6 +2150,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.60599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2161,6 +2281,106 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-BC79-E445-BC67-FD5EFE649D6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BSD_T_length '!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BSD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BSD_T_length '!$B$35:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BSD_T_length '!$B$44:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85199999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A38E-DD4D-9A30-145F4CBD52FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3266,28 +3486,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.5999999999999999E-2</c:v>
+                  <c:v>3.5999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16400000000000001</c:v>
+                  <c:v>0.17199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31</c:v>
+                  <c:v>0.35199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47799999999999998</c:v>
+                  <c:v>0.52200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66200000000000003</c:v>
+                  <c:v>0.71799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82399999999999995</c:v>
+                  <c:v>0.83599999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.89800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.94199999999999995</c:v>
+                  <c:v>0.92800000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4498,28 +4718,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                  <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.112</c:v>
+                  <c:v>8.4000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22600000000000001</c:v>
+                  <c:v>0.252</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35399999999999998</c:v>
+                  <c:v>0.374</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45800000000000002</c:v>
+                  <c:v>0.54600000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56799999999999995</c:v>
+                  <c:v>0.60399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63</c:v>
+                  <c:v>0.66200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67800000000000005</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4815,7 +5035,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$50</c:f>
+              <c:f>BSD_length!$A$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4838,7 +5058,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4871,34 +5091,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$50:$I$50</c:f>
+              <c:f>BSD_length!$B$47:$I$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2E-3</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4914,7 +5110,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$51</c:f>
+              <c:f>BSD_length!$A$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4937,7 +5133,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4970,34 +5166,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$51:$I$51</c:f>
+              <c:f>BSD_length!$B$48:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.8000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.3999999999999997E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5013,7 +5185,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$52</c:f>
+              <c:f>BSD_length!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5036,7 +5208,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5069,34 +5241,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$52:$I$52</c:f>
+              <c:f>BSD_length!$B$49:$I$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.5999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.7999999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.106</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.192</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.248</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.35599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.436</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5112,7 +5260,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$53</c:f>
+              <c:f>BSD_length!$A$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5135,7 +5283,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5168,34 +5316,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$53:$I$53</c:f>
+              <c:f>BSD_length!$B$50:$I$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.8000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.1999999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.17799999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.28000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.51</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.59199999999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.68400000000000005</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5211,7 +5335,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$54</c:f>
+              <c:f>BSD_length!$A$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5234,7 +5358,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5267,34 +5391,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$54:$I$54</c:f>
+              <c:f>BSD_length!$B$51:$I$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.5999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.17199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.33400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.54400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.754</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.82399999999999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.86199999999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5310,7 +5410,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$55</c:f>
+              <c:f>BSD_length!$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5333,7 +5433,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5366,34 +5466,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$55:$I$55</c:f>
+              <c:f>BSD_length!$B$52:$I$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.122</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.442</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.72199999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.85199999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.93600000000000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.95399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.96199999999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.95199999999999996</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5409,7 +5485,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$56</c:f>
+              <c:f>BSD_length!$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5434,7 +5510,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5467,34 +5543,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$56:$I$56</c:f>
+              <c:f>BSD_length!$B$53:$I$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.34599999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.79600000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.94599999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.98399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.97</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.98399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.96399999999999997</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5510,7 +5562,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>BSD_length!$A$57</c:f>
+              <c:f>BSD_length!$A$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5534,7 +5586,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BSD_length!$B$49:$I$49</c:f>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5567,7 +5619,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BSD_length!$B$57:$I$57</c:f>
+              <c:f>BSD_length!$B$54:$I$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5602,6 +5654,207 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-6834-0940-A63C-3ADD722AF8EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD_length!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Turns</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD_length!$B$55:$I$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.108</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.182</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5905-FE4D-897F-6C8C9990B7EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BSD_length!$A$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BSD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSD_length!$B$46:$I$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSD_length!$B$56:$I$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.50600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57399999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5905-FE4D-897F-6C8C9990B7EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6804,28 +7057,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3999999999999996E-2</c:v>
+                  <c:v>7.8E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.152</c:v>
+                  <c:v>0.14599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20200000000000001</c:v>
+                  <c:v>0.26200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.314</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.44</c:v>
+                  <c:v>0.47199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.53200000000000003</c:v>
+                  <c:v>0.55800000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.59799999999999998</c:v>
+                  <c:v>0.64400000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10532,13 +10785,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10902,8 +11155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11158,28 +11411,28 @@
         <v>8</v>
       </c>
       <c r="B14" s="3">
-        <v>4.2000000000000003E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="C14" s="3">
-        <v>0.31</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="D14" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="E14" s="3">
-        <v>0.77800000000000002</v>
+        <v>0.82</v>
       </c>
       <c r="F14" s="3">
-        <v>0.86399999999999999</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="G14" s="3">
-        <v>0.93200000000000005</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="H14" s="3">
-        <v>0.95799999999999996</v>
+        <v>0.96</v>
       </c>
       <c r="I14" s="3">
-        <v>0.96</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -11432,28 +11685,28 @@
         <v>8</v>
       </c>
       <c r="B28" s="18">
-        <v>4.5999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="C28" s="18">
-        <v>0.16400000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="D28" s="18">
-        <v>0.31</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="E28" s="18">
-        <v>0.47799999999999998</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="F28" s="18">
-        <v>0.66200000000000003</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="G28" s="18">
-        <v>0.82399999999999995</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="H28" s="18">
         <v>0.89800000000000002</v>
       </c>
       <c r="I28" s="18">
-        <v>0.94199999999999995</v>
+        <v>0.92800000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -11548,106 +11801,204 @@
       <c r="A38" s="8">
         <v>70</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="B38" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0.216</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0.434</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="G38" s="9">
+        <v>0.87</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="I38" s="9">
+        <v>0.92600000000000005</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>75</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
+      <c r="B39" s="4">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0.97</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>80</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
+      <c r="B40" s="3">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0.97799999999999998</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>90</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="B41" s="3">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.996</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0.98799999999999999</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>100</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
+      <c r="B42" s="3">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.998</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0.996</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0.98799999999999999</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="3">
         <v>0.16</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="3">
         <v>0.36</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="3">
         <v>0.60599999999999998</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="3">
         <v>0.73599999999999999</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>0.86399999999999999</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>0.90800000000000003</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="3">
         <v>0.93</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="3">
         <v>0.93799999999999994</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+      <c r="A44" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0.59</v>
+      </c>
+      <c r="F44" s="9">
+        <v>0.71</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="I44" s="9">
+        <v>0.85199999999999998</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
@@ -11674,10 +12025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A6:I58"/>
+  <dimension ref="A6:I56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11958,28 +12309,28 @@
         <v>8</v>
       </c>
       <c r="B17" s="12">
-        <v>0.03</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="C17" s="12">
-        <v>0.112</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="D17" s="12">
-        <v>0.22600000000000001</v>
+        <v>0.252</v>
       </c>
       <c r="E17" s="12">
-        <v>0.35399999999999998</v>
+        <v>0.374</v>
       </c>
       <c r="F17" s="12">
-        <v>0.45800000000000002</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="G17" s="12">
-        <v>0.56799999999999995</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="H17" s="12">
-        <v>0.63</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="I17" s="12">
-        <v>0.67800000000000005</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -12255,371 +12606,265 @@
         <v>8</v>
       </c>
       <c r="B34" s="3">
-        <v>1.7999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="C34" s="3">
-        <v>7.3999999999999996E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="D34" s="3">
-        <v>0.152</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="E34" s="3">
-        <v>0.20200000000000001</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="F34" s="3">
-        <v>0.314</v>
+        <v>0.35</v>
       </c>
       <c r="G34" s="3">
-        <v>0.44</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="H34" s="3">
-        <v>0.53200000000000003</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="I34" s="3">
-        <v>0.59799999999999998</v>
+        <v>0.64400000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
     </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+      <c r="B46" s="1">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1">
+        <v>10</v>
+      </c>
+      <c r="D46" s="1">
+        <v>15</v>
+      </c>
+      <c r="E46" s="1">
+        <v>20</v>
+      </c>
+      <c r="F46" s="1">
+        <v>25</v>
+      </c>
+      <c r="G46" s="1">
+        <v>30</v>
+      </c>
+      <c r="H46" s="1">
+        <v>35</v>
+      </c>
+      <c r="I46" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
+      <c r="A47" s="2">
+        <v>50</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
+    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>60</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="1">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1">
-        <v>10</v>
-      </c>
-      <c r="D49" s="1">
-        <v>15</v>
-      </c>
-      <c r="E49" s="1">
-        <v>20</v>
-      </c>
-      <c r="F49" s="1">
-        <v>25</v>
-      </c>
-      <c r="G49" s="1">
-        <v>30</v>
-      </c>
-      <c r="H49" s="1">
-        <v>35</v>
-      </c>
-      <c r="I49" s="1">
-        <v>40</v>
-      </c>
+    <row r="49" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>70</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>50</v>
-      </c>
-      <c r="B50" s="3">
-        <v>0</v>
-      </c>
-      <c r="C50" s="3">
-        <v>0</v>
-      </c>
-      <c r="D50" s="3">
-        <v>0</v>
-      </c>
-      <c r="E50" s="3">
-        <v>0</v>
-      </c>
-      <c r="F50" s="3">
-        <v>0</v>
-      </c>
-      <c r="G50" s="3">
-        <v>0</v>
-      </c>
-      <c r="H50" s="3">
-        <v>0</v>
-      </c>
-      <c r="I50" s="3">
-        <v>2E-3</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>60</v>
-      </c>
-      <c r="B51" s="3">
-        <v>0</v>
-      </c>
-      <c r="C51" s="3">
-        <v>0</v>
-      </c>
-      <c r="D51" s="3">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E51" s="3">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F51" s="3">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G51" s="3">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="H51" s="3">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="I51" s="3">
-        <v>4.3999999999999997E-2</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>70</v>
-      </c>
-      <c r="B52" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C52" s="3">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="D52" s="3">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="E52" s="3">
-        <v>0.106</v>
-      </c>
-      <c r="F52" s="3">
-        <v>0.192</v>
-      </c>
-      <c r="G52" s="3">
-        <v>0.248</v>
-      </c>
-      <c r="H52" s="3">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="I52" s="3">
-        <v>0.436</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>75</v>
-      </c>
-      <c r="B53" s="3">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="C53" s="3">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="D53" s="3">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="E53" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F53" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G53" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="H53" s="3">
-        <v>0.59199999999999997</v>
-      </c>
-      <c r="I53" s="3">
-        <v>0.68400000000000005</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>80</v>
-      </c>
-      <c r="B54" s="3">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="C54" s="3">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="D54" s="3">
-        <v>0.33400000000000002</v>
-      </c>
-      <c r="E54" s="3">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="F54" s="3">
-        <v>0.68</v>
-      </c>
-      <c r="G54" s="3">
-        <v>0.754</v>
-      </c>
-      <c r="H54" s="3">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="I54" s="3">
-        <v>0.86199999999999999</v>
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>0.11</v>
+      </c>
+      <c r="C54">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="D54">
+        <v>0.442</v>
+      </c>
+      <c r="E54">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="F54">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="G54">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="H54">
+        <v>0.85</v>
+      </c>
+      <c r="I54">
+        <v>0.84199999999999997</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
-        <v>90</v>
-      </c>
-      <c r="B55" s="3">
-        <v>0.122</v>
-      </c>
-      <c r="C55" s="3">
-        <v>0.442</v>
-      </c>
-      <c r="D55" s="3">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="E55" s="3">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="F55" s="3">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="G55" s="3">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="H55" s="3">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="I55" s="3">
-        <v>0.95199999999999996</v>
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>2E-3</v>
+      </c>
+      <c r="C55">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D55">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E55">
+        <v>0.108</v>
+      </c>
+      <c r="F55">
+        <v>0.182</v>
+      </c>
+      <c r="G55">
+        <v>0.27</v>
+      </c>
+      <c r="H55">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="I55">
+        <v>0.48799999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
-        <v>100</v>
-      </c>
-      <c r="B56" s="3">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="C56" s="3">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="D56" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="E56" s="3">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="F56" s="3">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="G56" s="3">
-        <v>0.97</v>
-      </c>
-      <c r="H56" s="3">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="I56" s="3">
-        <v>0.96399999999999997</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57">
-        <v>0.11</v>
-      </c>
-      <c r="C57">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="D57">
-        <v>0.442</v>
-      </c>
-      <c r="E57">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="F57">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="G57">
-        <v>0.81599999999999995</v>
-      </c>
-      <c r="H57">
-        <v>0.85</v>
-      </c>
-      <c r="I57">
-        <v>0.84199999999999997</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58">
-        <v>2E-3</v>
-      </c>
-      <c r="C58">
-        <v>1.6E-2</v>
-      </c>
-      <c r="D58">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="E58">
-        <v>0.108</v>
-      </c>
-      <c r="F58">
-        <v>0.182</v>
-      </c>
-      <c r="G58">
-        <v>0.27</v>
-      </c>
-      <c r="H58">
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="I58">
-        <v>0.48799999999999999</v>
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="7">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="C56" s="7">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.222</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="F56" s="7">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="H56" s="7">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="I56" s="7">
+        <v>0.57399999999999995</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="A45:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
plots for different classifiers
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39355D9-CBE8-1E49-A77F-7046FDFB0D15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976F2AB4-0FBB-BF4D-B416-F40F7106B479}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="460" windowWidth="24700" windowHeight="14220" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11340" yWindow="460" windowWidth="24700" windowHeight="14220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSD_T_length " sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,6 +218,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12928,8 +12932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12941,17 +12945,17 @@
       <c r="A1" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -13166,7 +13170,7 @@
       <c r="D12" s="17">
         <v>0.66200000000000003</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="12">
         <v>0.82</v>
       </c>
       <c r="F12" s="17">
@@ -13318,17 +13322,17 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
@@ -13631,7 +13635,7 @@
       <c r="D37" s="17">
         <v>0.32600000000000001</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="12">
         <v>0.52400000000000002</v>
       </c>
       <c r="F37" s="17">
@@ -13773,16 +13777,16 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
@@ -13998,7 +14002,7 @@
       <c r="D56" s="18">
         <v>0.44</v>
       </c>
-      <c r="E56" s="18">
+      <c r="E56" s="21">
         <v>0.59</v>
       </c>
       <c r="F56" s="18">
@@ -14146,8 +14150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A6:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14156,17 +14160,17 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
@@ -14494,7 +14498,7 @@
       <c r="D19" s="17">
         <v>0.246</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="12">
         <v>0.376</v>
       </c>
       <c r="F19" s="17">
@@ -14571,17 +14575,17 @@
     <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
@@ -14851,7 +14855,7 @@
       <c r="D37" s="17">
         <v>0.14599999999999999</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="12">
         <v>0.26200000000000001</v>
       </c>
       <c r="F37" s="17">
@@ -14996,17 +15000,17 @@
       <c r="I47"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
@@ -15197,7 +15201,7 @@
       <c r="D59" s="19">
         <v>0.222</v>
       </c>
-      <c r="E59" s="19">
+      <c r="E59" s="22">
         <v>0.32400000000000001</v>
       </c>
       <c r="F59" s="19">

</xml_diff>